<commit_message>
Fixed AntiSlip. Added requested features and refractored code.
</commit_message>
<xml_diff>
--- a/TiaAddin-Spin-ExcelReader/z.Excel Configurations/ConfigAllarmiUtenze.xlsx
+++ b/TiaAddin-Spin-ExcelReader/z.Excel Configurations/ConfigAllarmiUtenze.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PARONETTO G\Documents\GitHub\TiaAddIn-Spin\TiaAddin-Spin-ExcelReader\z.Excel Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE826CDE-B464-4369-94C8-128E1DFB875C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B86292-25AD-4905-81EC-E20859A467EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27750" windowHeight="16440" xr2:uid="{22A793F4-95FD-4AFA-8F43-DC77A5638B57}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{22A793F4-95FD-4AFA-8F43-DC77A5638B57}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="130">
-  <si>
-    <t>Descrizione allarme</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="140">
   <si>
     <t>Utenze</t>
   </si>
@@ -84,9 +81,6 @@
     <t>{user_name}.</t>
   </si>
   <si>
-    <t>Descrizione</t>
-  </si>
-  <si>
     <t>T#0s</t>
   </si>
   <si>
@@ -117,9 +111,6 @@
     <t>FC</t>
   </si>
   <si>
-    <t>Numero allarme</t>
-  </si>
-  <si>
     <t>Valori default campi</t>
   </si>
   <si>
@@ -141,9 +132,6 @@
     <t>Formato</t>
   </si>
   <si>
-    <t>Num. Partenza</t>
-  </si>
-  <si>
     <t>Salta ogni fine gruppo</t>
   </si>
   <si>
@@ -402,26 +390,72 @@
     <t>EstrusoreC Dosatore8</t>
   </si>
   <si>
-    <t>UnoPerSegmento</t>
-  </si>
-  <si>
     <t>Alm{alarm_num} - {user_description} {alarm_description}</t>
   </si>
   <si>
     <t>Alm{alarm_num_start} ~ {alarm_num_end} - {user_description}</t>
   </si>
   <si>
-    <t>Divisione uno alla volta</t>
-  </si>
-  <si>
-    <t>Divisione per gruppo</t>
+    <t>Generazione allarmi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nome &gt; {user_name} </t>
+  </si>
+  <si>
+    <t>Descrizione &gt; {user_description}</t>
+  </si>
+  <si>
+    <t>Num. Partenza &gt; {alarm_num}</t>
+  </si>
+  <si>
+    <t>Descrizione allarme &gt; {alarm_description}</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>Genera bobina prima di set</t>
+  </si>
+  <si>
+    <t>Divisione uno per segmento</t>
+  </si>
+  <si>
+    <t>GruppoPerSegmento</t>
+  </si>
+  <si>
+    <t>Divisione gruppo per segmento</t>
+  </si>
+  <si>
+    <t>(Solo per allarmi vuoti)</t>
+  </si>
+  <si>
+    <t>Alm{alarm_num} - SPARE</t>
+  </si>
+  <si>
+    <t>Alm{alarm_num_start} ~ {alarm_num_end} - SPARE</t>
+  </si>
+  <si>
+    <t>Lista Placeholders</t>
+  </si>
+  <si>
+    <t>Spare fine blocco</t>
+  </si>
+  <si>
+    <t>Indirizzo contatto spare</t>
+  </si>
+  <si>
+    <t>Genera vuoti in anti slittamento</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -482,6 +516,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -491,7 +532,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -561,11 +602,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
@@ -583,9 +651,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
@@ -602,11 +667,9 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -615,15 +678,39 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Migliaia" xfId="1" builtinId="3"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -936,667 +1023,724 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{667AB657-9EF0-4E7D-B211-0DE4E07AFF8D}">
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
     <col min="3" max="3" width="77.5703125" style="2" customWidth="1"/>
     <col min="4" max="4" width="1.7109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="33" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="37.42578125" style="2" customWidth="1"/>
     <col min="7" max="7" width="1.42578125" style="2" customWidth="1"/>
     <col min="8" max="11" width="20.7109375" style="2" customWidth="1"/>
     <col min="12" max="12" width="5.7109375" style="6" customWidth="1"/>
     <col min="13" max="13" width="8.7109375" style="6" customWidth="1"/>
-    <col min="14" max="14" width="45.7109375" style="6" customWidth="1"/>
+    <col min="14" max="14" width="49.85546875" style="6" customWidth="1"/>
     <col min="15" max="15" width="5.7109375" style="2" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="M1" s="7"/>
+      <c r="B1" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
     </row>
     <row r="2" spans="1:15" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="E2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="15"/>
+      <c r="H2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="E2" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="17"/>
-      <c r="H2" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
     </row>
     <row r="3" spans="1:15" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+    </row>
+    <row r="4" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
-    </row>
-    <row r="4" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="15"/>
+      <c r="C4" s="23"/>
       <c r="E4" s="3" t="s">
-        <v>2</v>
+        <v>124</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="N4" s="3" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="O4" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="O5" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="9" t="s">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="12">
+        <v>200</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N6" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N7" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E8" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N5" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="11">
-        <v>200</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N6" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E7" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N7" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="F8" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N8" s="19" t="s">
-        <v>63</v>
+        <v>24</v>
+      </c>
+      <c r="N8" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="O8" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>125</v>
+        <v>23</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N9" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N10" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N11" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C12" s="17"/>
+      <c r="E12" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N12" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" s="26">
+        <v>1002</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N9" s="19" t="s">
+      <c r="K13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N13" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="O9" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="2" t="s">
+      <c r="O13" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="K10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N10" s="19" t="s">
+      <c r="K14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N14" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="O10" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B11" s="14" t="s">
+      <c r="O14" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="12">
+        <v>25</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N15" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="12">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N16" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="O16" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B17" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N17" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="O17" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B18" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="C18" s="21">
+        <v>20</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N18" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="O18" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N19" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="O19" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N20" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="O20" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="23"/>
+      <c r="E21" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B22" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B23" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="E11" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N11" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="O11" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="8" t="s">
+      <c r="C23" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B24" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B25" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E27" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="23"/>
+      <c r="E28" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B29" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="13">
-        <v>1000</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N12" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="O12" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="8" t="s">
+      <c r="C29" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B30" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="8"/>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B31" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="8"/>
+    </row>
+    <row r="32" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="11"/>
+    </row>
+    <row r="33" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="2:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N13" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="O13" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="13">
-        <v>16</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N14" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="O14" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="11">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N15" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="O15" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E16" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N16" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="O16" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B17" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="15"/>
-      <c r="E17" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N17" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="O17" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N18" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="O18" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N19" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="O19" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N20" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="O20" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="22" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="23" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="24" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B24" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="15"/>
-      <c r="E24" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F25" s="2" t="s">
+      <c r="C34" s="23"/>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C35" s="8" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="9"/>
-      <c r="E26" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F26" s="2" t="s">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C37" s="8" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" s="9"/>
-      <c r="E27" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="28" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28" s="12"/>
-      <c r="E28" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="29" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B30" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" s="15"/>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B31" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="32" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>127</v>
+    <row r="38" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C1:O1"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B21:C21"/>
     <mergeCell ref="H3:O3"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B1:K1"/>
     <mergeCell ref="H2:O2"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{F5E4D3FC-4D67-4AB1-A3E0-2BD5870384F2}">
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{F5E4D3FC-4D67-4AB1-A3E0-2BD5870384F2}">
       <formula1>"UnoPerSegmento,GruppoPerSegmento"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12 C6 C14" xr:uid="{F717952B-D4F9-4570-84C1-F92597681F3D}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13 C6 C15" xr:uid="{F717952B-D4F9-4570-84C1-F92597681F3D}">
       <formula1>0</formula1>
       <formula2>99999</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{28CE5F0A-4030-43FD-81FB-F3DA458AE77A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{28CE5F0A-4030-43FD-81FB-F3DA458AE77A}">
       <formula1>"PerUtenza,PerTipoAllarme"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15" xr:uid="{7DFC26E2-A127-47D5-9AFB-DCB3CF89BE1E}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16" xr:uid="{7DFC26E2-A127-47D5-9AFB-DCB3CF89BE1E}">
       <formula1>0</formula1>
       <formula2>9999</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C21 L5:L1048576" xr:uid="{30675AF6-6451-470D-BF1D-59341B028670}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C25 L5:L1048576" xr:uid="{30675AF6-6451-470D-BF1D-59341B028670}">
       <formula1>"TON,TOF"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O5:O1048576" xr:uid="{ABA14625-FEA0-4BF2-8F91-7CEA04EDBD43}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O5:O1048576 C7 C17" xr:uid="{ABA14625-FEA0-4BF2-8F91-7CEA04EDBD43}">
       <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18" xr:uid="{273591C9-BB99-4728-86AC-9A463379FFFC}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>